<commit_message>
Updated Date Time technical notes
</commit_message>
<xml_diff>
--- a/zztechnotes/JulianDay/JulianDayTests_02.xlsx
+++ b/zztechnotes/JulianDay/JulianDayTests_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\datetimeopsgo\zztechnotes\JulianDay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95068950-9BA4-4DCF-83CE-A51DB26280A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814D56C-7364-4CD9-9692-4578F1D7F6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="4065" windowWidth="27915" windowHeight="9600" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
+    <workbookView xWindow="10905" yWindow="2085" windowWidth="27915" windowHeight="9600" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,70 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Nanosecond</t>
+  </si>
+  <si>
+    <t>JD for</t>
+  </si>
+  <si>
+    <t>Gregorian</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Day 0 of the first JD epoch</t>
+  </si>
+  <si>
+    <t>Midnight Next Day after zero</t>
+  </si>
+  <si>
+    <t>Midnight 12-hours before noon on day zero</t>
+  </si>
+  <si>
+    <t>2456293.520833333333333333315263297125</t>
+  </si>
+  <si>
+    <t>2458992.7468807870370370370453894093287772193434648215770721435546875000000000</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>2459007.301041666666666666663052659425</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000000000000000000000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,8 +125,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +455,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78ED6C8F-1928-4D54-91B3-A5407C84C1F2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="12.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="39.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="79.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>-4713</v>
+      </c>
+      <c r="C4" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>-4713</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>-4713</v>
+      </c>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2456293.5208333302</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>55</v>
+      </c>
+      <c r="G8" s="2">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2">
+        <v>500000000</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2458992.74688078</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2459007.3010416599</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on Gregorian Date to Juilain Date Conversion
</commit_message>
<xml_diff>
--- a/zztechnotes/JulianDay/JulianDayTests_02.xlsx
+++ b/zztechnotes/JulianDay/JulianDayTests_02.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\datetimeopsgo\zztechnotes\JulianDay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814D56C-7364-4CD9-9692-4578F1D7F6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77A89FF-93F8-4B50-ADFD-92FD83F47E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="2085" windowWidth="27915" windowHeight="9600" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
+    <workbookView xWindow="0" yWindow="3660" windowWidth="27915" windowHeight="9600" activeTab="1" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="JulianHours" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -87,18 +88,31 @@
   </si>
   <si>
     <t>2459007.301041666666666666663052659425</t>
+  </si>
+  <si>
+    <t>Gregorian Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000000000000000000000000000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000000000000000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -125,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,14 +147,19 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78ED6C8F-1928-4D54-91B3-A5407C84C1F2}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -702,4 +721,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F791BEB4-3AD7-4068-9B40-25B28F03961F}">
+  <dimension ref="A2:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new type CalendarDateTime
</commit_message>
<xml_diff>
--- a/zztechnotes/JulianDay/JulianDayTests_02.xlsx
+++ b/zztechnotes/JulianDay/JulianDayTests_02.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\datetimeopsgo\zztechnotes\JulianDay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77A89FF-93F8-4B50-ADFD-92FD83F47E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE6D975-CCFD-4BA7-868A-AEEFBA8FBA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3660" windowWidth="27915" windowHeight="9600" activeTab="1" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
+    <workbookView xWindow="4950" yWindow="1620" windowWidth="27915" windowHeight="9600" activeTab="2" xr2:uid="{8F799427-AFBC-409D-8755-ACBDBD0B70AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="JulianHours" sheetId="2" r:id="rId2"/>
+    <sheet name="JulianDateToGregorian" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -91,6 +92,16 @@
   </si>
   <si>
     <t>Gregorian Time</t>
+  </si>
+  <si>
+    <t>https://sciencing.com/calculate-years-across-bc-ad-8433373.html</t>
+  </si>
+  <si>
+    <t>Multiply the result in Step 1 by 3/4.
+Subtract 5/4 from the result of Step 2.
+Drop any digits to the right of the decimal point. The result is the number of days to add to the Julian date to get its equivalent Gregorian value.
+For example, October 2, 1216, has the calculation 12x.75-1.25 = 7.75. Truncating gives 7 days. So a Julian date of October 2, 1216, is October 9, 1216.
+Handle BC dates with the same calculations, but first subtract a year. After then performing the calculations above, add the year back in. The reason for this is to maintain the linear relationship of the formula, since there is no 0 BC or 0 AD. 1 AD follows 1 BC.</t>
   </si>
 </sst>
 </file>
@@ -101,9 +112,9 @@
     <numFmt numFmtId="164" formatCode="0.000000000000000000000000000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000000000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +125,14 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,10 +155,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,9 +179,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -727,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F791BEB4-3AD7-4068-9B40-25B28F03961F}">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -865,4 +888,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F293FFE-66A2-4D19-9E4D-3095DDBB752C}">
+  <dimension ref="C3:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{8787A0C8-7845-45E2-9D78-778CEB3987B3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>